<commit_message>
Removido a coluna UF
</commit_message>
<xml_diff>
--- a/solicitações_v4.xlsx
+++ b/solicitações_v4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://servicenow-my.sharepoint.com/personal/glaucco_morais_servicenow_com/Documents/Treinamentos/BB Digital Week/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8030675B-034E-B64F-A55A-7FD0609AE6C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{8030675B-034E-B64F-A55A-7FD0609AE6C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A8C2C6EB-AAB7-EE4B-9BD2-5F24D266D91B}"/>
   <bookViews>
     <workbookView xWindow="90440" yWindow="2660" windowWidth="27640" windowHeight="16940" xr2:uid="{44103DDD-AE48-1545-A3AF-37FF323BAF02}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="166">
   <si>
     <t>Aberto por</t>
   </si>
@@ -79,9 +79,6 @@
   </si>
   <si>
     <t>Saindo de</t>
-  </si>
-  <si>
-    <t>UF</t>
   </si>
   <si>
     <t>Valor da Passagem</t>
@@ -979,10 +976,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECA23025-A024-574A-9250-5CA4646F3D43}">
-  <dimension ref="A1:Q57"/>
+  <dimension ref="A1:P57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="P1" sqref="P1:P1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="33.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1002,16 +999,15 @@
     <col min="13" max="13" width="14.5" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="3.1640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -1041,10 +1037,10 @@
         <v>9</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>10</v>
@@ -1055,2975 +1051,2804 @@
       <c r="P1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:16" ht="34" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" ht="34" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="B2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="C2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="E2" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F2" s="6">
         <v>876.34</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H2" s="4">
         <v>45254</v>
       </c>
       <c r="I2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="4">
+        <v>45250</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="4">
-        <v>45250</v>
-      </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="L2" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="M2" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N2" s="7">
         <v>1</v>
       </c>
       <c r="O2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="P2" s="5">
+        <v>876.34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="P2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q2" s="5">
-        <v>876.34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="E3" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F3" s="6">
         <v>2931.22</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H3" s="4">
         <v>45254</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J3" s="4">
         <v>45250</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N3" s="7">
         <v>2</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q3" s="5">
+        <v>20</v>
+      </c>
+      <c r="P3" s="5">
         <v>2931.22</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="34" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="E4" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F4" s="6">
         <v>1467.89</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H4" s="4">
         <v>45254</v>
       </c>
       <c r="I4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="4">
+        <v>45250</v>
+      </c>
+      <c r="K4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="J4" s="4">
-        <v>45250</v>
-      </c>
-      <c r="K4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="L4" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="M4" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N4" s="7">
         <v>3</v>
       </c>
       <c r="O4" t="s">
+        <v>25</v>
+      </c>
+      <c r="P4" s="5">
+        <v>1467.89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="P4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q4" s="5">
-        <v>1467.89</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="B5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>28</v>
-      </c>
       <c r="E5" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F5" s="6">
         <v>2685.45</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H5" s="4">
         <v>45254</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J5" s="4">
         <v>45250</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N5" s="7">
         <v>1</v>
       </c>
       <c r="O5" t="s">
+        <v>29</v>
+      </c>
+      <c r="P5" s="5">
+        <v>2685.45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="34" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="P5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q5" s="5">
-        <v>2685.45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" ht="34" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+      <c r="B6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>32</v>
-      </c>
       <c r="E6" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F6" s="6">
         <v>1778.56</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H6" s="4">
         <v>45254</v>
       </c>
       <c r="I6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" s="4">
+        <v>45250</v>
+      </c>
+      <c r="K6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="J6" s="4">
-        <v>45250</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="L6" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N6" s="7">
         <v>2</v>
       </c>
       <c r="O6" t="s">
+        <v>33</v>
+      </c>
+      <c r="P6" s="5">
+        <v>1778.56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="P6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q6" s="5">
-        <v>1778.56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+      <c r="B7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>36</v>
-      </c>
       <c r="E7" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F7" s="6">
         <v>694.28</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H7" s="4">
         <v>45254</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J7" s="4">
         <v>45250</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N7" s="7">
         <v>3</v>
       </c>
       <c r="O7" t="s">
+        <v>37</v>
+      </c>
+      <c r="P7" s="5">
+        <v>694.28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="P7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q7" s="5">
-        <v>694.28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
+      <c r="B8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>40</v>
-      </c>
       <c r="E8" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F8" s="6">
         <v>3402.17</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H8" s="4">
         <v>45254</v>
       </c>
       <c r="I8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8" s="4">
+        <v>45250</v>
+      </c>
+      <c r="K8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="J8" s="4">
-        <v>45250</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="L8" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N8" s="7">
         <v>1</v>
       </c>
       <c r="O8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P8" s="5">
+        <v>3402.17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="P8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q8" s="5">
-        <v>3402.17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
+      <c r="B9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>44</v>
-      </c>
       <c r="E9" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F9" s="6">
         <v>1250.73</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H9" s="4">
         <v>45254</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J9" s="4">
         <v>45250</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N9" s="7">
         <v>2</v>
       </c>
       <c r="O9" t="s">
+        <v>45</v>
+      </c>
+      <c r="P9" s="5">
+        <v>1250.73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="34" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="P9" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q9" s="5">
-        <v>1250.73</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
+      <c r="B10" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="C10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="E10" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F10" s="6">
         <v>2176.98</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H10" s="4">
         <v>45254</v>
       </c>
       <c r="I10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" s="4">
+        <v>45250</v>
+      </c>
+      <c r="K10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="J10" s="4">
-        <v>45250</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="L10" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N10" s="7">
         <v>3</v>
       </c>
       <c r="O10" t="s">
+        <v>50</v>
+      </c>
+      <c r="P10" s="5">
+        <v>2176.98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="P10" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q10" s="5">
-        <v>2176.98</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
+      <c r="B11" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>53</v>
-      </c>
       <c r="E11" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F11" s="6">
         <v>3811.12</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H11" s="4">
         <v>45254</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J11" s="4">
         <v>45250</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N11" s="7">
         <v>1</v>
       </c>
       <c r="O11" t="s">
+        <v>54</v>
+      </c>
+      <c r="P11" s="5">
+        <v>3811.12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="P11" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q11" s="5">
-        <v>3811.12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" ht="34" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+      <c r="B12" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>57</v>
-      </c>
       <c r="E12" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F12" s="6">
         <v>1984.65</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H12" s="4">
         <v>45254</v>
       </c>
       <c r="I12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J12" s="4">
+        <v>45250</v>
+      </c>
+      <c r="K12" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="J12" s="4">
-        <v>45250</v>
-      </c>
-      <c r="K12" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="L12" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N12" s="7">
         <v>2</v>
       </c>
       <c r="O12" t="s">
+        <v>58</v>
+      </c>
+      <c r="P12" s="5">
+        <v>1984.65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="P12" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q12" s="5">
-        <v>1984.65</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>60</v>
-      </c>
       <c r="B13" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F13" s="6">
         <v>789.01</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H13" s="4">
         <v>45254</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J13" s="4">
         <v>45250</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N13" s="7">
         <v>3</v>
       </c>
       <c r="O13" t="s">
+        <v>61</v>
+      </c>
+      <c r="P13" s="5">
+        <v>789.01</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="34" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="P13" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q13" s="5">
-        <v>789.01</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" ht="34" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
+      <c r="B14" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>64</v>
-      </c>
       <c r="E14" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F14" s="6">
         <v>3056.43</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H14" s="4">
         <v>45254</v>
       </c>
       <c r="I14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J14" s="4">
+        <v>45250</v>
+      </c>
+      <c r="K14" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="J14" s="4">
-        <v>45250</v>
-      </c>
-      <c r="K14" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="L14" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N14" s="7">
         <v>1</v>
       </c>
       <c r="O14" t="s">
+        <v>65</v>
+      </c>
+      <c r="P14" s="5">
+        <v>3056.43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="P14" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q14" s="5">
-        <v>3056.43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>67</v>
-      </c>
       <c r="B15" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F15" s="6">
         <v>2345.67</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H15" s="4">
         <v>45254</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J15" s="4">
         <v>45250</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N15" s="7">
         <v>2</v>
       </c>
       <c r="O15" t="s">
+        <v>68</v>
+      </c>
+      <c r="P15" s="5">
+        <v>2345.67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="34" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="P15" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q15" s="5">
-        <v>2345.67</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" ht="34" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>70</v>
-      </c>
       <c r="B16" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F16" s="6">
         <v>1100.23</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H16" s="4">
         <v>45254</v>
       </c>
       <c r="I16" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J16" s="4">
+        <v>45250</v>
+      </c>
+      <c r="K16" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="J16" s="4">
-        <v>45250</v>
-      </c>
-      <c r="K16" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="L16" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N16" s="7">
         <v>3</v>
       </c>
       <c r="O16" t="s">
+        <v>71</v>
+      </c>
+      <c r="P16" s="5">
+        <v>1100.23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="P16" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q16" s="5">
-        <v>1100.23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>73</v>
-      </c>
       <c r="B17" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F17" s="6">
         <v>3698.76</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H17" s="4">
         <v>45254</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J17" s="4">
         <v>45250</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N17" s="7">
         <v>1</v>
       </c>
       <c r="O17" t="s">
+        <v>74</v>
+      </c>
+      <c r="P17" s="5">
+        <v>3698.76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="34" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="P17" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q17" s="5">
-        <v>3698.76</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" ht="34" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>76</v>
-      </c>
       <c r="B18" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F18" s="6">
         <v>1502.34</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H18" s="4">
         <v>45254</v>
       </c>
       <c r="I18" t="s">
+        <v>76</v>
+      </c>
+      <c r="J18" s="4">
+        <v>45250</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L18" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="J18" s="4">
-        <v>45250</v>
-      </c>
-      <c r="K18" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="L18" s="3" t="s">
-        <v>78</v>
-      </c>
       <c r="M18" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N18" s="7">
         <v>2</v>
       </c>
       <c r="O18" t="s">
-        <v>79</v>
-      </c>
-      <c r="P18" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q18" s="5">
+        <v>78</v>
+      </c>
+      <c r="P18" s="5">
         <v>1502.34</v>
       </c>
     </row>
-    <row r="19" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F19" s="6">
         <v>420.67</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H19" s="4">
         <v>45254</v>
       </c>
       <c r="I19" t="s">
+        <v>79</v>
+      </c>
+      <c r="J19" s="4">
+        <v>45250</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L19" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="J19" s="4">
-        <v>45250</v>
-      </c>
-      <c r="K19" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="L19" s="3" t="s">
-        <v>81</v>
-      </c>
       <c r="M19" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N19" s="7">
         <v>3</v>
       </c>
       <c r="O19" t="s">
+        <v>81</v>
+      </c>
+      <c r="P19" s="5">
+        <v>420.67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="34" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="P19" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q19" s="5">
-        <v>420.67</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" ht="34" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
+      <c r="B20" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>84</v>
-      </c>
       <c r="E20" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F20" s="6">
         <v>2765.43</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H20" s="4">
         <v>45254</v>
       </c>
       <c r="I20" t="s">
+        <v>84</v>
+      </c>
+      <c r="J20" s="4">
+        <v>45250</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L20" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="J20" s="4">
-        <v>45250</v>
-      </c>
-      <c r="K20" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="L20" s="3" t="s">
-        <v>86</v>
-      </c>
       <c r="M20" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N20" s="7">
         <v>1</v>
       </c>
       <c r="O20" t="s">
+        <v>86</v>
+      </c>
+      <c r="P20" s="5">
+        <v>2765.43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="P20" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q20" s="5">
-        <v>2765.43</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
-        <v>88</v>
-      </c>
       <c r="B21" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F21" s="6">
         <v>1892.76</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H21" s="4">
         <v>45254</v>
       </c>
       <c r="I21" t="s">
+        <v>88</v>
+      </c>
+      <c r="J21" s="4">
+        <v>45250</v>
+      </c>
+      <c r="K21" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L21" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="J21" s="4">
-        <v>45250</v>
-      </c>
-      <c r="K21" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="L21" s="3" t="s">
-        <v>90</v>
-      </c>
       <c r="M21" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N21" s="7">
         <v>2</v>
       </c>
       <c r="O21" t="s">
+        <v>90</v>
+      </c>
+      <c r="P21" s="5">
+        <v>1892.76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="34" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="P21" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q21" s="5">
-        <v>1892.76</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" ht="34" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
-        <v>92</v>
-      </c>
       <c r="B22" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="E22" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F22" s="6">
         <v>3499.88</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H22" s="4">
         <v>45254</v>
       </c>
       <c r="I22" t="s">
+        <v>92</v>
+      </c>
+      <c r="J22" s="4">
+        <v>45250</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L22" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="J22" s="4">
-        <v>45250</v>
-      </c>
-      <c r="K22" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="L22" s="3" t="s">
-        <v>94</v>
-      </c>
       <c r="M22" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N22" s="7">
         <v>3</v>
       </c>
       <c r="O22" t="s">
+        <v>94</v>
+      </c>
+      <c r="P22" s="5">
+        <v>3499.88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="P22" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q22" s="5">
-        <v>3499.88</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
-        <v>96</v>
-      </c>
       <c r="B23" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F23" s="6">
         <v>987.65</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H23" s="4">
         <v>45254</v>
       </c>
       <c r="I23" t="s">
+        <v>96</v>
+      </c>
+      <c r="J23" s="4">
+        <v>45250</v>
+      </c>
+      <c r="K23" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="J23" s="4">
-        <v>45250</v>
-      </c>
-      <c r="K23" s="3" t="s">
+      <c r="L23" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="L23" s="3" t="s">
-        <v>99</v>
-      </c>
       <c r="M23" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N23" s="7">
         <v>1</v>
       </c>
       <c r="O23" t="s">
+        <v>99</v>
+      </c>
+      <c r="P23" s="5">
+        <v>987.65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="P23" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q23" s="5">
-        <v>987.65</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
-        <v>101</v>
-      </c>
       <c r="B24" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F24" s="6">
         <v>2222.11</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H24" s="4">
         <v>45254</v>
       </c>
       <c r="I24" t="s">
+        <v>101</v>
+      </c>
+      <c r="J24" s="4">
+        <v>45250</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="L24" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="J24" s="4">
-        <v>45250</v>
-      </c>
-      <c r="K24" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="L24" s="3" t="s">
-        <v>103</v>
-      </c>
       <c r="M24" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N24" s="7">
         <v>2</v>
       </c>
       <c r="O24" t="s">
+        <v>103</v>
+      </c>
+      <c r="P24" s="5">
+        <v>2222.11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="P24" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q24" s="5">
-        <v>2222.11</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
-        <v>105</v>
-      </c>
       <c r="B25" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F25" s="6">
         <v>1567.89</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H25" s="4">
         <v>45254</v>
       </c>
       <c r="I25" t="s">
+        <v>105</v>
+      </c>
+      <c r="J25" s="4">
+        <v>45250</v>
+      </c>
+      <c r="K25" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L25" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="J25" s="4">
-        <v>45250</v>
-      </c>
-      <c r="K25" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="L25" s="3" t="s">
-        <v>107</v>
-      </c>
       <c r="M25" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N25" s="7">
         <v>3</v>
       </c>
       <c r="O25" t="s">
+        <v>107</v>
+      </c>
+      <c r="P25" s="5">
+        <v>1567.89</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" ht="34" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="P25" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q25" s="5">
-        <v>1567.89</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" ht="34" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
-        <v>109</v>
-      </c>
       <c r="B26" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F26" s="6">
         <v>431.2</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H26" s="4">
         <v>45254</v>
       </c>
       <c r="I26" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J26" s="4">
+        <v>45250</v>
+      </c>
+      <c r="K26" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="J26" s="4">
-        <v>45250</v>
-      </c>
-      <c r="K26" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="L26" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="M26" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N26" s="7">
         <v>1</v>
       </c>
       <c r="O26" t="s">
+        <v>110</v>
+      </c>
+      <c r="P26" s="5">
+        <v>431.2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="P26" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q26" s="5">
-        <v>431.2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
-        <v>112</v>
-      </c>
       <c r="B27" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F27" s="6">
         <v>2750.45</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H27" s="4">
         <v>45254</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J27" s="4">
         <v>45250</v>
       </c>
       <c r="K27" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="M27" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N27" s="7">
         <v>2</v>
       </c>
       <c r="O27" t="s">
+        <v>113</v>
+      </c>
+      <c r="P27" s="5">
+        <v>2750.45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="P27" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q27" s="5">
-        <v>2750.45</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
-        <v>115</v>
-      </c>
       <c r="B28" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F28" s="6">
         <v>1867.34</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H28" s="4">
         <v>45254</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J28" s="4">
         <v>45250</v>
       </c>
       <c r="K28" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L28" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M28" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N28" s="7">
         <v>3</v>
       </c>
       <c r="O28" t="s">
+        <v>116</v>
+      </c>
+      <c r="P28" s="5">
+        <v>1867.34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="P28" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q28" s="5">
-        <v>1867.34</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
-        <v>118</v>
-      </c>
       <c r="B29" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F29" s="6">
         <v>895.67</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H29" s="4">
         <v>45254</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J29" s="4">
         <v>45250</v>
       </c>
       <c r="K29" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L29" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M29" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N29" s="7">
         <v>1</v>
       </c>
       <c r="O29" t="s">
-        <v>119</v>
-      </c>
-      <c r="P29" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q29" s="5">
+        <v>118</v>
+      </c>
+      <c r="P29" s="5">
         <v>895.67</v>
       </c>
     </row>
-    <row r="30" spans="1:17" ht="34" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F30" s="6">
         <v>3276.54</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H30" s="4">
         <v>45254</v>
       </c>
       <c r="I30" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J30" s="4">
+        <v>45250</v>
+      </c>
+      <c r="K30" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="J30" s="4">
-        <v>45250</v>
-      </c>
-      <c r="K30" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="L30" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M30" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N30" s="7">
         <v>2</v>
       </c>
       <c r="O30" t="s">
+        <v>119</v>
+      </c>
+      <c r="P30" s="5">
+        <v>3276.54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="P30" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q30" s="5">
-        <v>3276.54</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
-        <v>121</v>
-      </c>
       <c r="B31" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F31" s="6">
         <v>1222.33</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H31" s="4">
         <v>45254</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J31" s="4">
         <v>45250</v>
       </c>
       <c r="K31" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L31" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M31" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N31" s="7">
         <v>3</v>
       </c>
       <c r="O31" t="s">
+        <v>121</v>
+      </c>
+      <c r="P31" s="5">
+        <v>1222.33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="P31" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q31" s="5">
-        <v>1222.33</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
+      <c r="B32" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="B32" s="3" t="s">
-        <v>124</v>
-      </c>
       <c r="C32" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F32" s="6">
         <v>2999.12</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H32" s="4">
         <v>45254</v>
       </c>
       <c r="I32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J32" s="4">
         <v>45250</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L32" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M32" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N32" s="7">
         <v>1</v>
       </c>
       <c r="O32" t="s">
-        <v>125</v>
-      </c>
-      <c r="P32" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q32" s="5">
+        <v>124</v>
+      </c>
+      <c r="P32" s="5">
         <v>2999.12</v>
       </c>
     </row>
-    <row r="33" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B33" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="B33" s="3" t="s">
-        <v>124</v>
-      </c>
       <c r="C33" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F33" s="6">
         <v>1456.78</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H33" s="4">
         <v>45254</v>
       </c>
       <c r="I33" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J33" s="4">
         <v>45250</v>
       </c>
       <c r="K33" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L33" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M33" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N33" s="7">
         <v>2</v>
       </c>
       <c r="O33" t="s">
+        <v>125</v>
+      </c>
+      <c r="P33" s="5">
+        <v>1456.78</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" ht="34" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="P33" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q33" s="5">
-        <v>1456.78</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17" ht="34" x14ac:dyDescent="0.2">
-      <c r="A34" s="3" t="s">
-        <v>127</v>
-      </c>
       <c r="B34" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F34" s="6">
         <v>3701.23</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H34" s="4">
         <v>45254</v>
       </c>
       <c r="I34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J34" s="4">
         <v>45250</v>
       </c>
       <c r="K34" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L34" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="M34" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N34" s="7">
         <v>3</v>
       </c>
       <c r="O34" t="s">
+        <v>128</v>
+      </c>
+      <c r="P34" s="5">
+        <v>3701.23</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="P34" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q34" s="5">
-        <v>3701.23</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
-        <v>130</v>
-      </c>
       <c r="B35" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F35" s="6">
         <v>545.66999999999996</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H35" s="4">
         <v>45254</v>
       </c>
       <c r="I35" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J35" s="4">
         <v>45250</v>
       </c>
       <c r="K35" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L35" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="M35" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N35" s="7">
         <v>1</v>
       </c>
       <c r="O35" t="s">
+        <v>131</v>
+      </c>
+      <c r="P35" s="5">
+        <v>545.66999999999996</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="P35" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q35" s="5">
-        <v>545.66999999999996</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="A36" s="3" t="s">
-        <v>133</v>
-      </c>
       <c r="B36" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F36" s="6">
         <v>2710.98</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H36" s="4">
         <v>45254</v>
       </c>
       <c r="I36" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J36" s="4">
         <v>45250</v>
       </c>
       <c r="K36" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L36" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M36" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N36" s="7">
         <v>2</v>
       </c>
       <c r="O36" t="s">
+        <v>133</v>
+      </c>
+      <c r="P36" s="5">
+        <v>2710.98</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="P36" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q36" s="5">
-        <v>2710.98</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="A37" s="3" t="s">
-        <v>135</v>
-      </c>
       <c r="B37" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F37" s="6">
         <v>967.89</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H37" s="4">
         <v>45254</v>
       </c>
       <c r="I37" t="s">
+        <v>96</v>
+      </c>
+      <c r="J37" s="4">
+        <v>45250</v>
+      </c>
+      <c r="K37" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="J37" s="4">
-        <v>45250</v>
-      </c>
-      <c r="K37" s="3" t="s">
-        <v>98</v>
-      </c>
       <c r="L37" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M37" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N37" s="7">
         <v>3</v>
       </c>
       <c r="O37" t="s">
+        <v>135</v>
+      </c>
+      <c r="P37" s="5">
+        <v>967.89</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="P37" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q37" s="5">
-        <v>967.89</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="A38" s="3" t="s">
-        <v>137</v>
-      </c>
       <c r="B38" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F38" s="6">
         <v>3911</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H38" s="4">
         <v>45254</v>
       </c>
       <c r="I38" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J38" s="4">
         <v>45250</v>
       </c>
       <c r="K38" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L38" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M38" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N38" s="7">
         <v>1</v>
       </c>
       <c r="O38" t="s">
+        <v>137</v>
+      </c>
+      <c r="P38" s="5">
+        <v>3911</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="P38" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q38" s="5">
-        <v>3911</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="A39" s="3" t="s">
-        <v>139</v>
-      </c>
       <c r="B39" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F39" s="6">
         <v>1589.12</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H39" s="4">
         <v>45254</v>
       </c>
       <c r="I39" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J39" s="4">
         <v>45250</v>
       </c>
       <c r="K39" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L39" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M39" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N39" s="7">
         <v>2</v>
       </c>
       <c r="O39" t="s">
+        <v>139</v>
+      </c>
+      <c r="P39" s="5">
+        <v>1589.12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A40" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="P39" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q39" s="5">
-        <v>1589.12</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="A40" s="3" t="s">
-        <v>141</v>
-      </c>
       <c r="B40" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F40" s="6">
         <v>340.22</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H40" s="4">
         <v>45254</v>
       </c>
       <c r="I40" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J40" s="4">
         <v>45250</v>
       </c>
       <c r="K40" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L40" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M40" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N40" s="7">
         <v>3</v>
       </c>
       <c r="O40" t="s">
+        <v>142</v>
+      </c>
+      <c r="P40" s="5">
+        <v>340.22</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A41" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="P40" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q40" s="5">
-        <v>340.22</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="A41" s="3" t="s">
-        <v>144</v>
-      </c>
       <c r="B41" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F41" s="6">
         <v>2987.65</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H41" s="4">
         <v>45254</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J41" s="4">
         <v>45250</v>
       </c>
       <c r="K41" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L41" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M41" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N41" s="7">
         <v>1</v>
       </c>
       <c r="O41" t="s">
+        <v>144</v>
+      </c>
+      <c r="P41" s="5">
+        <v>2987.65</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A42" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="P41" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q41" s="5">
-        <v>2987.65</v>
-      </c>
-    </row>
-    <row r="42" spans="1:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="A42" s="3" t="s">
-        <v>146</v>
-      </c>
       <c r="B42" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F42" s="6">
         <v>1734.56</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H42" s="4">
         <v>45254</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J42" s="4">
         <v>45250</v>
       </c>
       <c r="K42" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L42" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M42" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N42" s="7">
         <v>2</v>
       </c>
       <c r="O42" t="s">
-        <v>77</v>
-      </c>
-      <c r="P42" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q42" s="5">
+        <v>76</v>
+      </c>
+      <c r="P42" s="5">
         <v>1734.56</v>
       </c>
     </row>
-    <row r="43" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F43" s="6">
         <v>765.43</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H43" s="4">
         <v>45254</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J43" s="4">
         <v>45250</v>
       </c>
       <c r="K43" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L43" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M43" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N43" s="7">
         <v>3</v>
       </c>
       <c r="O43" t="s">
-        <v>80</v>
-      </c>
-      <c r="P43" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q43" s="5">
+        <v>79</v>
+      </c>
+      <c r="P43" s="5">
         <v>765.43</v>
       </c>
     </row>
-    <row r="44" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F44" s="6">
         <v>3456.78</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H44" s="4">
         <v>45254</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J44" s="4">
         <v>45250</v>
       </c>
       <c r="K44" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L44" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M44" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N44" s="7">
         <v>1</v>
       </c>
       <c r="O44" t="s">
-        <v>85</v>
-      </c>
-      <c r="P44" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q44" s="5">
+        <v>84</v>
+      </c>
+      <c r="P44" s="5">
         <v>3456.78</v>
       </c>
     </row>
-    <row r="45" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F45" s="6">
         <v>1122.33</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H45" s="4">
         <v>45254</v>
       </c>
       <c r="I45" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J45" s="4">
         <v>45250</v>
       </c>
       <c r="K45" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L45" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M45" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N45" s="7">
         <v>2</v>
       </c>
       <c r="O45" t="s">
-        <v>89</v>
-      </c>
-      <c r="P45" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q45" s="5">
+        <v>88</v>
+      </c>
+      <c r="P45" s="5">
         <v>1122.33</v>
       </c>
     </row>
-    <row r="46" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F46" s="6">
         <v>2389</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H46" s="4">
         <v>45254</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J46" s="4">
         <v>45250</v>
       </c>
       <c r="K46" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L46" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M46" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N46" s="7">
         <v>3</v>
       </c>
       <c r="O46" t="s">
-        <v>93</v>
-      </c>
-      <c r="P46" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q46" s="5">
+        <v>92</v>
+      </c>
+      <c r="P46" s="5">
         <v>2389</v>
       </c>
     </row>
-    <row r="47" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F47" s="6">
         <v>1845.67</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H47" s="4">
         <v>45254</v>
       </c>
       <c r="I47" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J47" s="4">
         <v>45250</v>
       </c>
       <c r="K47" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L47" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="M47" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N47" s="7">
         <v>1</v>
       </c>
       <c r="O47" t="s">
-        <v>97</v>
-      </c>
-      <c r="P47" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q47" s="5">
+        <v>96</v>
+      </c>
+      <c r="P47" s="5">
         <v>1845.67</v>
       </c>
     </row>
-    <row r="48" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F48" s="6">
         <v>690.12</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H48" s="4">
         <v>45254</v>
       </c>
       <c r="I48" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J48" s="4">
         <v>45250</v>
       </c>
       <c r="K48" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L48" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M48" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N48" s="7">
         <v>2</v>
       </c>
       <c r="O48" t="s">
-        <v>102</v>
-      </c>
-      <c r="P48" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q48" s="5">
+        <v>101</v>
+      </c>
+      <c r="P48" s="5">
         <v>690.12</v>
       </c>
     </row>
-    <row r="49" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F49" s="6">
         <v>3555.22</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H49" s="4">
         <v>45254</v>
       </c>
       <c r="I49" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J49" s="4">
         <v>45250</v>
       </c>
       <c r="K49" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="L49" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="L49" s="3" t="s">
-        <v>99</v>
-      </c>
       <c r="M49" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N49" s="7">
         <v>3</v>
       </c>
       <c r="O49" t="s">
-        <v>106</v>
-      </c>
-      <c r="P49" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q49" s="5">
+        <v>105</v>
+      </c>
+      <c r="P49" s="5">
         <v>3555.22</v>
       </c>
     </row>
-    <row r="50" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F50" s="6">
         <v>1344.56</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H50" s="4">
         <v>45254</v>
       </c>
       <c r="I50" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J50" s="4">
         <v>45250</v>
       </c>
       <c r="K50" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L50" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M50" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N50" s="7">
         <v>1</v>
       </c>
       <c r="O50" t="s">
-        <v>142</v>
-      </c>
-      <c r="P50" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q50" s="5">
+        <v>141</v>
+      </c>
+      <c r="P50" s="5">
         <v>1344.56</v>
       </c>
     </row>
-    <row r="51" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F51" s="6">
         <v>2221</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H51" s="4">
         <v>45254</v>
       </c>
       <c r="I51" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J51" s="4">
         <v>45250</v>
       </c>
       <c r="K51" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L51" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M51" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N51" s="7">
         <v>2</v>
       </c>
       <c r="O51" t="s">
-        <v>151</v>
-      </c>
-      <c r="P51" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q51" s="5">
+        <v>150</v>
+      </c>
+      <c r="P51" s="5">
         <v>2221</v>
       </c>
     </row>
-    <row r="52" spans="1:17" ht="34" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F52" s="6">
         <v>1122.33</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H52" s="4">
         <v>45254</v>
       </c>
       <c r="I52" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J52" s="4">
         <v>45250</v>
       </c>
       <c r="K52" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L52" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="L52" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="M52" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N52" s="7">
         <v>3</v>
       </c>
       <c r="O52" t="s">
-        <v>153</v>
-      </c>
-      <c r="P52" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="P52" s="5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A53" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D53" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="Q52" s="5">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="53" spans="1:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="A53" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="E53" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F53" s="6">
         <v>2389</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H53" s="4">
         <v>45254</v>
       </c>
       <c r="I53" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J53" s="4">
         <v>45250</v>
       </c>
       <c r="K53" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L53" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M53" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N53" s="7">
         <v>1</v>
       </c>
       <c r="O53" t="s">
-        <v>155</v>
-      </c>
-      <c r="P53" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="P53" s="5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" ht="34" x14ac:dyDescent="0.2">
+      <c r="A54" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D54" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="Q53" s="5">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="54" spans="1:17" ht="34" x14ac:dyDescent="0.2">
-      <c r="A54" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="E54" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F54" s="6">
         <v>1845.67</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H54" s="4">
         <v>45254</v>
       </c>
       <c r="I54" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J54" s="4">
+        <v>45250</v>
+      </c>
+      <c r="K54" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="J54" s="4">
-        <v>45250</v>
-      </c>
-      <c r="K54" s="3" t="s">
+      <c r="L54" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="L54" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="M54" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N54" s="7">
         <v>2</v>
       </c>
       <c r="O54" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="P54" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="P54" s="5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A55" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D55" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="Q54" s="5">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="55" spans="1:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="A55" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D55" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="E55" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F55" s="6">
         <v>690.12</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H55" s="4">
         <v>45254</v>
       </c>
       <c r="I55" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J55" s="4">
         <v>45250</v>
       </c>
       <c r="K55" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L55" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M55" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N55" s="7">
         <v>3</v>
       </c>
       <c r="O55" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="P55" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="P55" s="5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" ht="34" x14ac:dyDescent="0.2">
+      <c r="A56" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D56" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="Q55" s="5">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="56" spans="1:17" ht="34" x14ac:dyDescent="0.2">
-      <c r="A56" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D56" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="E56" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F56" s="6">
         <v>3555.22</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H56" s="4">
         <v>45254</v>
       </c>
       <c r="I56" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J56" s="4">
+        <v>45250</v>
+      </c>
+      <c r="K56" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="J56" s="4">
-        <v>45250</v>
-      </c>
-      <c r="K56" s="3" t="s">
+      <c r="L56" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="L56" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="M56" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N56" s="7">
         <v>2</v>
       </c>
       <c r="O56" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="P56" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="P56" s="5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A57" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D57" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="Q56" s="5">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="57" spans="1:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="A57" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D57" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="E57" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F57" s="6">
         <v>1344.56</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H57" s="4">
         <v>45254</v>
       </c>
       <c r="I57" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J57" s="4">
         <v>45250</v>
       </c>
       <c r="K57" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L57" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M57" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N57" s="7">
         <v>2</v>
       </c>
       <c r="O57" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="P57" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q57" s="5">
+        <v>20</v>
+      </c>
+      <c r="P57" s="5">
         <v>100</v>
       </c>
     </row>

</xml_diff>